<commit_message>
push code 20-6 18:55
</commit_message>
<xml_diff>
--- a/Source/OMT/Equipment/Datasheet/DATASHEET - Hạ Vy/DATASHEET.xlsx
+++ b/Source/OMT/Equipment/Datasheet/DATASHEET - Hạ Vy/DATASHEET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DATASHEET - Hạ Vy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B18FFFF-843C-401E-A772-37783A71CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C291E9B0-FFCF-40E5-8932-4BC424ABBC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="847" activeTab="1" xr2:uid="{EF4B7A21-D4C5-4932-9D03-30F4F8AD3AC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="847" activeTab="4" xr2:uid="{EF4B7A21-D4C5-4932-9D03-30F4F8AD3AC6}"/>
   </bookViews>
   <sheets>
     <sheet name="CẢM BIẾN QUANG" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="143">
   <si>
     <t xml:space="preserve"> Mã cảm biến</t>
   </si>
@@ -270,9 +270,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.2 MPa - 1 MPa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.1 MPa - 1 MPa</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.15 MPa - 1 MPa</t>
@@ -476,6 +473,21 @@
   </si>
   <si>
     <t>đại ca mở phút thứ 5 lên sẽ thấy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CDM2B40 - 200Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TN10X60S  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 160 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 200 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.05 MPa - 1 MPa </t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1190,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1222,7 +1234,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="4:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1255,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1263,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1271,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1279,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1287,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="4:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1295,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1311,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="4:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D0A639-CF2E-4410-860E-2E514A2328B4}">
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+    <sheetView zoomScale="98" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1342,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1350,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1358,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1366,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1374,7 +1386,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1382,15 +1394,15 @@
         <v>6</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1398,20 +1410,20 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" t="s">
         <v>135</v>
-      </c>
-      <c r="E10" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1438,117 +1450,117 @@
         <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
         <v>79</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1577,15 +1589,15 @@
         <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="2:3" s="18" customFormat="1" ht="79.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="2:3" s="18" customFormat="1" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1593,7 +1605,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="2:3" s="18" customFormat="1" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1601,31 +1613,31 @@
         <v>37</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="18" customFormat="1" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:3" s="18" customFormat="1" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="18" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1642,22 +1654,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A410198-0340-4C37-9F26-176BB1FFC47A}">
-  <dimension ref="B1:E35"/>
+  <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="53" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:E34"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1666,8 +1680,14 @@
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1676,8 +1696,14 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1686,8 +1712,14 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1696,8 +1728,14 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1708,20 +1746,26 @@
       <c r="E6" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="2:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1730,8 +1774,14 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1740,8 +1790,14 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1750,8 +1806,14 @@
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1760,8 +1822,14 @@
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
@@ -1770,20 +1838,26 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="2:5" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="19.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="1" t="s">
@@ -1810,7 +1884,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1872,7 +1946,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1902,7 +1976,7 @@
         <v>19</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1918,7 +1992,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1926,7 +2000,7 @@
         <v>23</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="4:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1934,7 +2008,7 @@
         <v>26</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="4:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -2089,7 +2163,7 @@
         <v>57</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2132,7 +2206,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2140,7 +2214,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>